<commit_message>
feat(FN-3616): add csv with empty entries e2e-test
</commit_message>
<xml_diff>
--- a/e2e-tests/ukef/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
+++ b/e2e-tests/ukef/cypress/fixtures/valid-utilisation-report-February_2023_monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RLavender\Work\dtfs2\e2e-tests\ukef\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58607CB-0BB6-4060-8284-39A9E0D54731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C1C776-6A1C-4ADD-B4B0-F6B3EC26FF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29650" yWindow="-21730" windowWidth="38620" windowHeight="21100" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Bank facility reference</t>
   </si>
@@ -95,16 +95,19 @@
     <t>Total fees accrued for the period</t>
   </si>
   <si>
-    <t>total fees accrued for the period currency</t>
-  </si>
-  <si>
-    <t>total fees accrued for the period exchange rate</t>
-  </si>
-  <si>
     <t>Column for notes for devs - DO NOT leave notes at the end of rows we have special handling around end of rows that needs testing</t>
   </si>
   <si>
     <t>This line is included to test empty optional columns parsed correctly when they are the final entry in the row</t>
+  </si>
+  <si>
+    <t>accrual exchange rate</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>accrual currency</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -572,15 +575,15 @@
         <v>16</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -683,7 +686,7 @@
         <v>1.17</v>
       </c>
       <c r="M4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="N4">
         <v>1.17</v>

</xml_diff>